<commit_message>
sapflow per ground area over time plots
</commit_message>
<xml_diff>
--- a/Data/Processed/Daytime/Models.xlsx
+++ b/Data/Processed/Daytime/Models.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yliua\Desktop\MP.June\Data\Processed\Daytime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2799D241-C192-4373-9894-58F66A91B0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1729C4-CDF2-403A-B4AF-C6C4192ABD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2895" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="2" r:id="rId1"/>
-    <sheet name="Q2" sheetId="3" r:id="rId2"/>
-    <sheet name="Q3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Q2" sheetId="3" r:id="rId3"/>
+    <sheet name="Q3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="97">
   <si>
     <t>DenstyL:GnO</t>
   </si>
@@ -137,12 +138,6 @@
     <t>df</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Std.</t>
-  </si>
-  <si>
     <t>Estimate</t>
   </si>
   <si>
@@ -303,16 +298,44 @@
   </si>
   <si>
     <t>976,</t>
+  </si>
+  <si>
+    <t>Std. Error</t>
+  </si>
+  <si>
+    <t>H(0)</t>
+  </si>
+  <si>
+    <t>L(1)</t>
+  </si>
+  <si>
+    <t>A(0)</t>
+  </si>
+  <si>
+    <t>B(1)</t>
+  </si>
+  <si>
+    <t>C(2)</t>
+  </si>
+  <si>
+    <t>O(3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -326,7 +349,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -334,13 +357,166 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +844,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,103 +856,103 @@
   <sheetData>
     <row r="2" spans="1:14" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
         <v>70</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>69</v>
       </c>
-      <c r="J3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K3" t="s">
-        <v>71</v>
-      </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>1892.8</v>
@@ -784,27 +960,27 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -826,29 +1002,29 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
@@ -862,7 +1038,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -876,7 +1052,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>8.0379000000000006E-2</v>
@@ -887,88 +1063,115 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I17">
         <v>4</v>
       </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" t="s">
         <v>32</v>
       </c>
+      <c r="J20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" s="15">
+        <v>0</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="12">
         <v>2.2086700000000001</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="12">
         <v>6.3619999999999996E-2</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="12">
         <v>36.757800000000003</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="12">
         <v>34.719000000000001</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="13">
         <v>2E-16</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="14" t="s">
         <v>27</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K21" s="15">
+        <v>0</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -996,6 +1199,15 @@
       <c r="H22" t="s">
         <v>27</v>
       </c>
+      <c r="J22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K22" s="15">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1021,6 +1233,15 @@
       </c>
       <c r="H23" t="s">
         <v>27</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" s="17">
+        <v>0</v>
+      </c>
+      <c r="L23" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -1359,11 +1580,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188D256B-9522-4C0B-8A5C-4456293B6463}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1977B83-A602-417F-8B51-6483C4C25C1A}">
   <dimension ref="A2:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E16"/>
+      <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1375,109 +1610,109 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
         <v>70</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>69</v>
       </c>
-      <c r="L3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" t="s">
-        <v>71</v>
-      </c>
       <c r="N3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>1830.9</v>
@@ -1485,27 +1720,27 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1527,29 +1762,29 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
@@ -1563,7 +1798,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -1577,7 +1812,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>8.0379000000000006E-2</v>
@@ -1588,28 +1823,28 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I17">
         <v>4</v>
@@ -1620,29 +1855,26 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2113,12 +2345,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2BBBD3-A326-4619-9F79-F4936C420D68}">
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2130,103 +2362,103 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" t="s">
         <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>498.9</v>
@@ -2234,71 +2466,71 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="B9">
         <v>-3.3942000000000001</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>-0.54969999999999997</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>-1.6000000000000001E-3</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.56630000000000003</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>4.6517999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
@@ -2312,7 +2544,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14">
         <v>6.3369999999999996E-2</v>
@@ -2323,22 +2555,22 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G15">
         <v>122</v>
@@ -2349,29 +2581,26 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2397,6 +2626,7 @@
       <c r="H19" t="s">
         <v>27</v>
       </c>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -2527,7 +2757,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B25">
         <v>0.70145999999999997</v>
@@ -2620,7 +2850,7 @@
         <v>1.89E-2</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -2706,7 +2936,7 @@
         <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I33" t="s">
         <v>9</v>
@@ -2787,7 +3017,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B39">
         <v>-0.55100000000000005</v>
@@ -2897,5 +3127,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
graphs and mp report
</commit_message>
<xml_diff>
--- a/Data/Processed/Daytime/Models.xlsx
+++ b/Data/Processed/Daytime/Models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yliua\Desktop\MP.June\Data\Processed\Daytime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5026CD61-1533-448D-B498-52317566B448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09715A0-A087-44D0-AAC4-F837F40C2EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2895" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Sheet3" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="134">
   <si>
     <t>DenstyL:GnO</t>
   </si>
@@ -390,6 +389,48 @@
   </si>
   <si>
     <t>1|BlockTRUE</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>SoMo</t>
+  </si>
+  <si>
+    <t>Density:SoMo</t>
+  </si>
+  <si>
+    <t>Geno:SoMo</t>
+  </si>
+  <si>
+    <t>Density:Geno:SoMo</t>
+  </si>
+  <si>
+    <t>m&lt;-aov(SapflowPerGroundArea</t>
+  </si>
+  <si>
+    <t>Density*Geno*SoMo+</t>
+  </si>
+  <si>
+    <t>(1|</t>
+  </si>
+  <si>
+    <t>+(1|Block),</t>
+  </si>
+  <si>
+    <t>Low)</t>
+  </si>
+  <si>
+    <t>+ (1|DOY)</t>
+  </si>
+  <si>
+    <t>High)</t>
+  </si>
+  <si>
+    <t>Wet</t>
+  </si>
+  <si>
+    <t>Dry</t>
   </si>
 </sst>
 </file>
@@ -549,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -589,6 +630,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,20 +694,25 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>967740</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>586741</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7958823" cy="4236720"/>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>392637</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>149929</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3820C95B-42E5-4877-A36B-52E31A535EE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C642BCDA-EB41-228F-13B7-417C1E9ADA48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -681,8 +728,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="967740" y="3019425"/>
-          <a:ext cx="7958823" cy="4236720"/>
+          <a:off x="586741" y="9128760"/>
+          <a:ext cx="5307536" cy="3274129"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -690,7 +737,95 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>27412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>383893</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>50869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A868C6C-E543-28AF-1BF4-FC677757D51C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="9171412"/>
+          <a:ext cx="5077813" cy="3132417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>229857</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>7209</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7667C6AA-EDA0-7923-6AA8-83858F9A1657}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6278880" y="0"/>
+          <a:ext cx="11934177" cy="5493609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -959,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30BD2C4-1BF8-489F-8700-1BE1FEF7BF83}">
   <dimension ref="A2:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1697,21 +1832,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A54D916-79F1-4DBB-91EF-29C550261392}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1992,6 +2129,747 @@
       </c>
       <c r="J14">
         <v>7.1312920000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>424.1</v>
+      </c>
+      <c r="D19">
+        <v>424.1</v>
+      </c>
+      <c r="E19">
+        <v>1047.9269999999999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2E-16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>74.5</v>
+      </c>
+      <c r="D20">
+        <v>24.8</v>
+      </c>
+      <c r="E20">
+        <v>61.405999999999999</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2E-16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>51.4</v>
+      </c>
+      <c r="D21">
+        <v>25.7</v>
+      </c>
+      <c r="E21">
+        <v>63.488999999999997</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2E-16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>139.1</v>
+      </c>
+      <c r="D22">
+        <v>46.4</v>
+      </c>
+      <c r="E22">
+        <v>114.613</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2E-16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>9.9390000000000001</v>
+      </c>
+      <c r="G23" s="1">
+        <v>4.9499999999999997E-5</v>
+      </c>
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>16.7</v>
+      </c>
+      <c r="D24">
+        <v>2.8</v>
+      </c>
+      <c r="E24">
+        <v>6.8579999999999997</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2.96E-7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>8.4</v>
+      </c>
+      <c r="D25">
+        <v>1.4</v>
+      </c>
+      <c r="E25">
+        <v>3.444</v>
+      </c>
+      <c r="G25">
+        <v>2.15E-3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26">
+        <v>3880</v>
+      </c>
+      <c r="C26">
+        <v>1570.1</v>
+      </c>
+      <c r="D26">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <v>1E-3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <v>0.01</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28">
+        <v>0.05</v>
+      </c>
+      <c r="J28" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28">
+        <v>0.1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" t="s">
+        <v>103</v>
+      </c>
+      <c r="K31" t="s">
+        <v>104</v>
+      </c>
+      <c r="L31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M31" t="s">
+        <v>74</v>
+      </c>
+      <c r="N31" t="s">
+        <v>73</v>
+      </c>
+      <c r="O31" t="s">
+        <v>72</v>
+      </c>
+      <c r="P31" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q31" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" t="s">
+        <v>129</v>
+      </c>
+      <c r="J32" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" t="s">
+        <v>67</v>
+      </c>
+      <c r="L32" t="s">
+        <v>105</v>
+      </c>
+      <c r="M32" t="s">
+        <v>106</v>
+      </c>
+      <c r="N32" t="s">
+        <v>104</v>
+      </c>
+      <c r="O32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" t="s">
+        <v>109</v>
+      </c>
+      <c r="K34" t="s">
+        <v>108</v>
+      </c>
+      <c r="L34" t="s">
+        <v>113</v>
+      </c>
+      <c r="M34" t="s">
+        <v>114</v>
+      </c>
+      <c r="N34" t="s">
+        <v>120</v>
+      </c>
+      <c r="O34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>226.4</v>
+      </c>
+      <c r="D35">
+        <v>226.39</v>
+      </c>
+      <c r="E35">
+        <v>632.42999999999995</v>
+      </c>
+      <c r="F35" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J35" t="s">
+        <v>73</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>93.23</v>
+      </c>
+      <c r="M35">
+        <v>93.23</v>
+      </c>
+      <c r="N35">
+        <v>252.065</v>
+      </c>
+      <c r="O35" t="s">
+        <v>28</v>
+      </c>
+      <c r="P35" s="1">
+        <v>2E-16</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>47.5</v>
+      </c>
+      <c r="D36">
+        <v>15.84</v>
+      </c>
+      <c r="E36">
+        <v>44.26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K36">
+        <v>3</v>
+      </c>
+      <c r="L36">
+        <v>14.93</v>
+      </c>
+      <c r="M36">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="N36">
+        <v>13.455</v>
+      </c>
+      <c r="O36" s="1">
+        <v>1.6499999999999999E-8</v>
+      </c>
+      <c r="P36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>121</v>
+      </c>
+      <c r="D37">
+        <v>40.33</v>
+      </c>
+      <c r="E37">
+        <v>112.65</v>
+      </c>
+      <c r="F37" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" t="s">
+        <v>27</v>
+      </c>
+      <c r="J37" t="s">
+        <v>111</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>6.54</v>
+      </c>
+      <c r="M37">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="N37">
+        <v>5.8940000000000001</v>
+      </c>
+      <c r="O37">
+        <v>5.7300000000000005E-4</v>
+      </c>
+      <c r="P37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38">
+        <v>2484</v>
+      </c>
+      <c r="C38">
+        <v>889.2</v>
+      </c>
+      <c r="D38">
+        <v>0.36</v>
+      </c>
+      <c r="J38" t="s">
+        <v>112</v>
+      </c>
+      <c r="K38">
+        <v>604</v>
+      </c>
+      <c r="L38">
+        <v>223.4</v>
+      </c>
+      <c r="M38">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40">
+        <v>1E-3</v>
+      </c>
+      <c r="O40" t="s">
+        <v>20</v>
+      </c>
+      <c r="P40">
+        <v>0.01</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>19</v>
+      </c>
+      <c r="R40">
+        <v>0.05</v>
+      </c>
+      <c r="S40" t="s">
+        <v>18</v>
+      </c>
+      <c r="T40">
+        <v>0.1</v>
+      </c>
+      <c r="U40" t="s">
+        <v>17</v>
+      </c>
+      <c r="V40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2.0340043900000002</v>
+      </c>
+      <c r="B44">
+        <v>-0.61583138000000004</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.35958243000000001</v>
+      </c>
+      <c r="D44">
+        <v>-0.69684787999999998</v>
+      </c>
+      <c r="E44" s="2">
+        <v>4.4466520000000002E-2</v>
+      </c>
+      <c r="F44">
+        <v>-0.50278630999999996</v>
+      </c>
+      <c r="G44">
+        <v>0.71461134000000004</v>
+      </c>
+      <c r="H44">
+        <v>-9.4942520000000002E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2.5015872300000002</v>
+      </c>
+      <c r="B47">
+        <v>-1.01055446</v>
+      </c>
+      <c r="C47" s="2">
+        <v>-6.5165459999999995E-2</v>
+      </c>
+      <c r="D47">
+        <v>-0.54093859</v>
+      </c>
+      <c r="E47" s="2">
+        <v>-0.25543274999999999</v>
+      </c>
+      <c r="F47">
+        <v>-0.19168661000000001</v>
+      </c>
+      <c r="G47">
+        <v>0.43165297000000002</v>
+      </c>
+      <c r="H47">
+        <v>0.32348942000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>